<commit_message>
added final touches and design document
</commit_message>
<xml_diff>
--- a/TraceabilityMatrix.xlsx
+++ b/TraceabilityMatrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Problemo\Documents\Work\School work\Year 4\Winter 2024\3004 Software Engineering\Assignments\A3\qt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Problemo\Documents\Work\School work\Year 4\Winter 2024\3004 Software Engineering\Assignments\A3VM\3004A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10918009-9DAC-44EA-9DD8-40C865EE4A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7B3775-A281-4FA7-9739-58A11532B710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{75ECCB6F-E88A-48F5-AD64-D8A34769466F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -149,57 +149,12 @@
     <t>1,2,3,4,5,6</t>
   </si>
   <si>
-    <t>Button, Elevator</t>
-  </si>
-  <si>
     <t>Elevator</t>
   </si>
   <si>
-    <t>Button</t>
-  </si>
-  <si>
-    <t>Door</t>
-  </si>
-  <si>
-    <t>Door,ECS</t>
-  </si>
-  <si>
-    <t>Button,ECS, Door</t>
-  </si>
-  <si>
-    <t>Elevator, ECS</t>
-  </si>
-  <si>
-    <t>ECS</t>
-  </si>
-  <si>
-    <t>Button,ECS</t>
-  </si>
-  <si>
-    <t>ECS,Door,Elevator</t>
-  </si>
-  <si>
-    <t>ECS,Elevator</t>
-  </si>
-  <si>
-    <t>ECS,Elevator,Door</t>
-  </si>
-  <si>
-    <t>Button,Door</t>
-  </si>
-  <si>
-    <t>Elevator,Floor,Door,Button,ECS</t>
-  </si>
-  <si>
-    <t>Floor,Button</t>
-  </si>
-  <si>
     <t>Implemented By</t>
   </si>
   <si>
-    <t>Fulfilled by</t>
-  </si>
-  <si>
     <t>MainWindow, ECS, Elevator</t>
   </si>
   <si>
@@ -216,6 +171,45 @@
   </si>
   <si>
     <t>Elevator,ECS,MainWindow</t>
+  </si>
+  <si>
+    <t>Tested by</t>
+  </si>
+  <si>
+    <t>Pressing floor buttons simultaneously</t>
+  </si>
+  <si>
+    <t>Pressing any floor button</t>
+  </si>
+  <si>
+    <t>Pressing floor button, then pressing elevator button</t>
+  </si>
+  <si>
+    <t>N/A - part of GUI</t>
+  </si>
+  <si>
+    <t>Pressing open/close doors button</t>
+  </si>
+  <si>
+    <t>Pressing the help button</t>
+  </si>
+  <si>
+    <t>Pressing any floor button, integrated into movement</t>
+  </si>
+  <si>
+    <t>Testing with floor button then elevator button</t>
+  </si>
+  <si>
+    <t>Pressing the door obstacle button</t>
+  </si>
+  <si>
+    <t>Pressing the fire button</t>
+  </si>
+  <si>
+    <t>Setting the weight of the passenger &gt;300 in the elevator.h class</t>
+  </si>
+  <si>
+    <t>Pressing the power outage button</t>
   </si>
 </sst>
 </file>
@@ -353,7 +347,7 @@
     <tableColumn id="1" xr3:uid="{A2D580E5-8848-49EA-9586-241BC29EA12C}" name="id" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{FFA1AC09-061D-4914-9072-E1BAE8A02FD4}" name="Requirement" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{549C6D59-DB2B-41A0-A8AC-77E760FE6B23}" name="Related Use Case"/>
-    <tableColumn id="4" xr3:uid="{92017525-1934-455D-8EF4-D1A073BE8A5D}" name="Fulfilled by"/>
+    <tableColumn id="4" xr3:uid="{92017525-1934-455D-8EF4-D1A073BE8A5D}" name="Tested by"/>
     <tableColumn id="5" xr3:uid="{112C989F-46A3-4AD1-A01F-AA75351DB509}" name="Implemented By"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -660,7 +654,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,10 +677,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -703,10 +697,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -720,10 +714,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -737,10 +731,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -754,10 +748,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -771,10 +765,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -788,10 +782,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -805,10 +799,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -822,10 +816,10 @@
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -839,10 +833,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -856,10 +850,10 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -873,10 +867,10 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -890,10 +884,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -907,10 +901,10 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -924,10 +918,10 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
@@ -941,10 +935,10 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
@@ -958,10 +952,10 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>